<commit_message>
Finalizado a insercao de statusrohs pelo XIM.
</commit_message>
<xml_diff>
--- a/fax/NOV'18_month.xlsx
+++ b/fax/NOV'18_month.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\Documents\NetBeansProjects\XRFSlave\fax\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5DBAE8D-B13D-4315-8EED-173BD3E28728}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="6705" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -391,9 +397,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-416]d\-mmm;@"/>
+    <numFmt numFmtId="164" formatCode="[$-416]d\-mmm;@"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -558,14 +564,14 @@
     <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -839,14 +845,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -875,40 +881,40 @@
   <sheetData>
     <row r="1" spans="1:14" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="17" t="s">
+      <c r="H1" s="18" t="s">
         <v>121</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="16" t="s">
+      <c r="K1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="16" t="s">
+      <c r="L1" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="16" t="s">
+      <c r="M1" s="17" t="s">
         <v>10</v>
       </c>
       <c r="N1" s="2" t="s">
@@ -917,18 +923,18 @@
     </row>
     <row r="2" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
       <c r="N2" s="1" t="s">
         <v>12</v>
       </c>
@@ -943,7 +949,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
       <c r="G3" s="7"/>
-      <c r="H3" s="18">
+      <c r="H3" s="16">
         <v>43405</v>
       </c>
       <c r="I3" s="14" t="s">
@@ -975,7 +981,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
       <c r="G4" s="8"/>
-      <c r="H4" s="18">
+      <c r="H4" s="16">
         <v>43405</v>
       </c>
       <c r="I4" s="14" t="s">
@@ -1007,7 +1013,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="15"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="18">
+      <c r="H5" s="16">
         <v>43405</v>
       </c>
       <c r="I5" s="14" t="s">
@@ -1039,7 +1045,7 @@
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="8"/>
-      <c r="H6" s="18">
+      <c r="H6" s="16">
         <v>43405</v>
       </c>
       <c r="I6" s="14" t="s">
@@ -1071,7 +1077,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="7"/>
-      <c r="H7" s="18">
+      <c r="H7" s="16">
         <v>43409</v>
       </c>
       <c r="I7" s="14" t="s">
@@ -1103,7 +1109,7 @@
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="8"/>
-      <c r="H8" s="18">
+      <c r="H8" s="16">
         <v>43410</v>
       </c>
       <c r="I8" s="14" t="s">
@@ -1135,7 +1141,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="7"/>
-      <c r="H9" s="18">
+      <c r="H9" s="16">
         <v>43410</v>
       </c>
       <c r="I9" s="14" t="s">
@@ -1167,7 +1173,7 @@
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="8"/>
-      <c r="H10" s="18">
+      <c r="H10" s="16">
         <v>43410</v>
       </c>
       <c r="I10" s="12" t="s">
@@ -1199,7 +1205,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="18">
+      <c r="H11" s="16">
         <v>43411</v>
       </c>
       <c r="I11" s="14" t="s">
@@ -1231,7 +1237,7 @@
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="8"/>
-      <c r="H12" s="18">
+      <c r="H12" s="16">
         <v>43414</v>
       </c>
       <c r="I12" s="12" t="s">
@@ -1263,7 +1269,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
       <c r="G13" s="7"/>
-      <c r="H13" s="18">
+      <c r="H13" s="16">
         <v>43414</v>
       </c>
       <c r="I13" s="14" t="s">
@@ -1295,7 +1301,7 @@
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="8"/>
-      <c r="H14" s="18">
+      <c r="H14" s="16">
         <v>43414</v>
       </c>
       <c r="I14" s="14" t="s">
@@ -1327,7 +1333,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="7"/>
-      <c r="H15" s="18">
+      <c r="H15" s="16">
         <v>43415</v>
       </c>
       <c r="I15" s="11" t="s">
@@ -1359,7 +1365,7 @@
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="8"/>
-      <c r="H16" s="18">
+      <c r="H16" s="16">
         <v>43416</v>
       </c>
       <c r="I16" s="12" t="s">
@@ -1391,7 +1397,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
       <c r="G17" s="7"/>
-      <c r="H17" s="18">
+      <c r="H17" s="16">
         <v>43417</v>
       </c>
       <c r="I17" s="14" t="s">
@@ -1423,7 +1429,7 @@
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="8"/>
-      <c r="H18" s="18">
+      <c r="H18" s="16">
         <v>43418</v>
       </c>
       <c r="I18" s="12" t="s">
@@ -1455,7 +1461,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
       <c r="G19" s="7"/>
-      <c r="H19" s="18">
+      <c r="H19" s="16">
         <v>43421</v>
       </c>
       <c r="I19" s="11" t="s">
@@ -1487,7 +1493,7 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="8"/>
-      <c r="H20" s="18">
+      <c r="H20" s="16">
         <v>43421</v>
       </c>
       <c r="I20" s="12" t="s">
@@ -1519,7 +1525,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
       <c r="G21" s="7"/>
-      <c r="H21" s="18">
+      <c r="H21" s="16">
         <v>43421</v>
       </c>
       <c r="I21" s="11" t="s">
@@ -1551,7 +1557,7 @@
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="18">
+      <c r="H22" s="16">
         <v>43422</v>
       </c>
       <c r="I22" s="14" t="s">
@@ -1583,7 +1589,7 @@
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="7"/>
-      <c r="H23" s="18">
+      <c r="H23" s="16">
         <v>43423</v>
       </c>
       <c r="I23" s="14" t="s">
@@ -1615,7 +1621,7 @@
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="8"/>
-      <c r="H24" s="18">
+      <c r="H24" s="16">
         <v>43424</v>
       </c>
       <c r="I24" s="12" t="s">
@@ -1647,7 +1653,7 @@
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
       <c r="G25" s="7"/>
-      <c r="H25" s="18">
+      <c r="H25" s="16">
         <v>43427</v>
       </c>
       <c r="I25" s="11" t="s">
@@ -1679,7 +1685,7 @@
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="8"/>
-      <c r="H26" s="18">
+      <c r="H26" s="16">
         <v>43427</v>
       </c>
       <c r="I26" s="12" t="s">
@@ -1711,7 +1717,7 @@
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
       <c r="G27" s="7"/>
-      <c r="H27" s="18">
+      <c r="H27" s="16">
         <v>43427</v>
       </c>
       <c r="I27" s="11" t="s">
@@ -1743,7 +1749,7 @@
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="8"/>
-      <c r="H28" s="18">
+      <c r="H28" s="16">
         <v>43428</v>
       </c>
       <c r="I28" s="14" t="s">
@@ -1775,7 +1781,7 @@
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="7"/>
-      <c r="H29" s="18">
+      <c r="H29" s="16">
         <v>43429</v>
       </c>
       <c r="I29" s="11" t="s">
@@ -1807,7 +1813,7 @@
       <c r="E30" s="6"/>
       <c r="F30" s="6"/>
       <c r="G30" s="8"/>
-      <c r="H30" s="18">
+      <c r="H30" s="16">
         <v>43433</v>
       </c>
       <c r="I30" s="12" t="s">
@@ -1839,7 +1845,7 @@
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="7"/>
-      <c r="H31" s="18">
+      <c r="H31" s="16">
         <v>43433</v>
       </c>
       <c r="I31" s="14" t="s">
@@ -1871,7 +1877,7 @@
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="8"/>
-      <c r="H32" s="18">
+      <c r="H32" s="16">
         <v>43433</v>
       </c>
       <c r="I32" s="14" t="s">
@@ -1903,7 +1909,7 @@
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="7"/>
-      <c r="H33" s="18">
+      <c r="H33" s="16">
         <v>43434</v>
       </c>
       <c r="I33" s="11" t="s">
@@ -1935,7 +1941,7 @@
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="8"/>
-      <c r="H34" s="18">
+      <c r="H34" s="16">
         <v>43434</v>
       </c>
       <c r="I34" s="12" t="s">

</xml_diff>